<commit_message>
Final No tocar nada mas
</commit_message>
<xml_diff>
--- a/Data/MatrizPrecisionesModelos.xlsx
+++ b/Data/MatrizPrecisionesModelos.xlsx
@@ -665,19 +665,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8178947368421052</v>
+        <v>0.8242105263157895</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7689423377106458</v>
+        <v>0.7674876618243893</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3159203980099503</v>
+        <v>0.3308457711442786</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1461949265687583</v>
+        <v>0.1341789052069426</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7617602703928185</v>
+        <v>0.7591655481289358</v>
       </c>
     </row>
     <row r="12">
@@ -687,19 +687,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8231578947368421</v>
+        <v>0.8215789473684211</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7613600887418714</v>
+        <v>0.7621787590751185</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3457711442786069</v>
+        <v>0.3407960199004975</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1315086782376502</v>
+        <v>0.1348464619492657</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7522934033367699</v>
+        <v>0.7534638409386557</v>
       </c>
     </row>
     <row r="13">
@@ -709,19 +709,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8315789473684211</v>
+        <v>0.8278947368421052</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7248404174056288</v>
+        <v>0.7006639034467184</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4601990049751244</v>
+        <v>0.5199004975124378</v>
       </c>
       <c r="E13" t="n">
-        <v>0.09012016021361816</v>
+        <v>0.0787716955941255</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7091802389220366</v>
+        <v>0.6819971899339645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>